<commit_message>
some pictures and tables were updated
</commit_message>
<xml_diff>
--- a/figures and tables/B.tables.xlsx
+++ b/figures and tables/B.tables.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="head_width" sheetId="1" r:id="rId1"/>
     <sheet name="dev.char" sheetId="2" r:id="rId2"/>
     <sheet name="mean.dev.time" sheetId="3" r:id="rId3"/>
+    <sheet name="List1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Instar</t>
   </si>
@@ -161,6 +162,33 @@
       <t>(means, standard errors and number of individuals).</t>
     </r>
   </si>
+  <si>
+    <t>Temperature range</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Df</t>
+  </si>
+  <si>
+    <t>p value</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k </t>
+  </si>
+  <si>
+    <t>15-21</t>
+  </si>
+  <si>
+    <t>15-25</t>
+  </si>
+  <si>
+    <t>Table 1: Summary of development constants for S. watsoni for five developmental stages  (sum of effective temperatures (k) and lower developmental threshold (t))  (means and standard errors).</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +284,18 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,6 +412,41 @@
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,9 +855,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -791,7 +868,7 @@
     <col min="5" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1">
       <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
@@ -801,7 +878,7 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
@@ -821,7 +898,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
@@ -841,7 +918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -861,7 +938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>28</v>
       </c>
@@ -881,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -889,12 +966,8 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+    <row r="8" spans="1:8">
+      <c r="H8" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -907,7 +980,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1062,4 +1135,186 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="30">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="D4" s="30">
+        <v>220</v>
+      </c>
+      <c r="E4" s="31">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="30">
+        <v>0.9375</v>
+      </c>
+      <c r="D5" s="30">
+        <v>171</v>
+      </c>
+      <c r="E5" s="31">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="D6" s="30">
+        <v>206</v>
+      </c>
+      <c r="E6" s="31">
+        <v>2.2E-16</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="32">
+        <v>0.81989999999999996</v>
+      </c>
+      <c r="D7" s="30">
+        <v>27</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1.4860000000000001E-11</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="34">
+        <v>0.85629999999999995</v>
+      </c>
+      <c r="D8" s="35">
+        <v>10</v>
+      </c>
+      <c r="E8" s="36">
+        <v>1.607E-5</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>